<commit_message>
Excel done with subregion and dispo
</commit_message>
<xml_diff>
--- a/epg_data.xlsx
+++ b/epg_data.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,34 +463,34 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>BRAVO TV</t>
+          <t>NET TV</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/BRAVOTV/EXPORTACION_WEB/SS/BRAVOTV_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/NETTV/EXPORTACION_WEB/SS/NETTV_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>NET TV</t>
+          <t>AMERICA TV</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/NETTV/EXPORTACION_WEB/SS/NETTV_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/AMERICATV/EXPORTACION_WEB/SS/AMERICATV_t-290x163.png</t>
         </is>
       </c>
     </row>
@@ -519,2403 +519,2556 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>TELEFÉ</t>
+          <t>CANAL 8 DE CÓRDOBA</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/TELEF/EXPORTACION_WEB/SS/TELEF_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/CANAL8DECRDOBA/EXPORTACION_WEB/SS/CANAL8DECRDOBA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>TV PÚBLICA ARGENTINA</t>
+          <t>TUCUMÁN 8</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/TVPBLICAARGENTINA/EXPORTACION_WEB/SS/TVPBLICAARGENTINA_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/TUCUMN8/EXPORTACION_WEB/SS/TUCUMN8_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>CANAL 9 INTERIOR</t>
+          <t>TELEFÉ</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/CANAL9INTERIOR/EXPORTACION_WEB/SS/CANAL9INTERIOR_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/TELEF/EXPORTACION_WEB/SS/TELEF_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>CANAL 9 MENDOZA</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/A24/EXPORTACION_WEB/SS/A24_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CANAL9MENDOZA/EXPORTACION_WEB/SS/CANAL9MENDOZA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>C5N HD</t>
+          <t>CANAL 5 DE ROSARIO</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/C5NHD/EXPORTACION_WEB/SS/C5NHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CANAL5DEROSARIO/EXPORTACION_WEB/SS/CANAL5DEROSARIO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>CRÓNICA TV HD</t>
+          <t>CANAL 13 DE SANTA FE</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/CRNICATVHD/EXPORTACION_WEB/SS/CRNICATVHD_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CANAL13DESANTAFE/EXPORTACION_WEB/SS/CANAL13DESANTAFE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>LA NACIÓN +</t>
+          <t>TELEFÉ MDQ</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/LANACIN/EXPORTACION_WEB/SS/LANACIN_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/TELEFMDQ/EXPORTACION_WEB/SS/TELEFMDQ_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>CANAL IP</t>
+          <t>TV PÚBLICA ARGENTINA</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/CANALIP/EXPORTACION_WEB/SS/CANALIP_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/TVPBLICAARGENTINA/EXPORTACION_WEB/SS/TVPBLICAARGENTINA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>CANAL 26</t>
+          <t>CANAL 9</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/CANAL26/EXPORTACION_WEB/SS/CANAL26_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CANAL9/EXPORTACION_WEB/SS/CANAL9_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>ENCUENTRO</t>
+          <t>CANAL 9 INTERIOR</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/ENCUENTRO/EXPORTACION_WEB/SS/ENCUENTRO_t-290x163.png</t>
+          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/CANAL9INTERIOR/EXPORTACION_WEB/SS/CANAL9INTERIOR_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>CANAL E</t>
+          <t>CANAL 13 : BUENOS AIRES</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CANALE/EXPORTACION_WEB/SS/CANALE_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CANAL13BUENOSAIRES/EXPORTACION_WEB/SS/CANAL13BUENOSAIRES_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>CANAL 4 EXTRA</t>
+          <t>CANAL 13 INTERIOR</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CANAL4EXTRA/EXPORTACION_WEB/SS/CANAL4EXTRA_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CANAL13INTERIOR/EXPORTACION_WEB/SS/CANAL13INTERIOR_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>DIPUTADOS TV ARG</t>
+          <t>CANAL 12 CÓRDOBA</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/DIPUTADOSTVARG/EXPORTACION_WEB/SS/DIPUTADOSTVARG_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CANAL12CRDOBA/EXPORTACION_WEB/SS/CANAL12CRDOBA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>MULTIVISION HD</t>
+          <t>CANAL 3 ROSARIO</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/MULTIVISIONHD/EXPORTACION_WEB/SS/MULTIVISIONHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CANAL3ROSARIO/EXPORTACION_WEB/SS/CANAL3ROSARIO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>T5 SATELITAL</t>
+          <t>CANAL 9 RESISTENCIA</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/T5SATELITAL/EXPORTACION_WEB/SS/T5SATELITAL_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/CANAL9RESISTENCIA/EXPORTACION_WEB/SS/CANAL9RESISTENCIA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>CANAL 12 MISIONES</t>
+          <t>CANAL 10 TUCUMÁN</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/CANAL12MISIONES/EXPORTACION_WEB/SS/CANAL12MISIONES_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CANAL10TUCUMN/EXPORTACION_WEB/SS/CANAL10TUCUMN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>TELEDIARIO</t>
+          <t>CANAL 10 MDQ</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/TELEDIARIO/EXPORTACION_WEB/SS/TELEDIARIO_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CANAL10MDQ/EXPORTACION_WEB/SS/CANAL10MDQ_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>NORTE GRANDE FEDERAL</t>
+          <t>CANAL TN</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/NORTEGRANDEFEDERAL/EXPORTACION_WEB/SS/NORTEGRANDEFEDERAL_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/CANALTN/EXPORTACION_WEB/SS/CANALTN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>CLARO SPORTS</t>
+          <t>AMÉRICA TUCUMÁN</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CLAROSPORTS/EXPORTACION_WEB/SS/CLAROSPORTS_t-290x163.png</t>
+          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/AMRICATUCUMN/EXPORTACION_WEB/SS/AMRICATUCUMN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>TYC SPORTS</t>
+          <t>A24</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/TYCSPORTS/EXPORTACION_WEB/SS/TYCSPORTS_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/A24/EXPORTACION_WEB/SS/A24_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>ESPN NEW</t>
+          <t>C5N HD</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/ESPNNEW/EXPORTACION_WEB/SS/ESPNNEW_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/C5NHD/EXPORTACION_WEB/SS/C5NHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>ESPN 2 NEW</t>
+          <t>CRÓNICA TV HD</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/ESPN2NEW/EXPORTACION_WEB/SS/ESPN2NEW_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CRNICATVHD/EXPORTACION_WEB/SS/CRNICATVHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>ESPN 3</t>
+          <t>LA NACIÓN +</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/ESPN3/EXPORTACION_WEB/SS/ESPN3_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/LANACIN/EXPORTACION_WEB/SS/LANACIN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>ESPN 4</t>
+          <t>CANAL IP</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/ESPN4/EXPORTACION_WEB/SS/ESPN4_t-290x163.png</t>
+          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/CANALIP/EXPORTACION_WEB/SS/CANALIP_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>FOX SPORTS NEW</t>
+          <t>ENCUENTRO</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/FOXSPORTSNEW/EXPORTACION_WEB/SS/FOXSPORTSNEW_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/ENCUENTRO/EXPORTACION_WEB/SS/ENCUENTRO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>FOX SPORTS 2 NEW</t>
+          <t>CANAL 4 EXTRA</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/FOXSPORTS2NEW/EXPORTACION_WEB/SS/FOXSPORTS2NEW_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CANAL4EXTRA/EXPORTACION_WEB/SS/CANAL4EXTRA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>FOX SPORTS 3 NEW</t>
+          <t>DIPUTADOS TV ARG</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/FOXSPORTS3NEW/EXPORTACION_WEB/SS/FOXSPORTS3NEW_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DIPUTADOSTVARG/EXPORTACION_WEB/SS/DIPUTADOSTVARG_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>DeporTV HD</t>
+          <t>CIUDAD MAGAZINE</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/DEPORTVHD/EXPORTACION_WEB/SS/DEPORTVHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/CIUDADMAGAZINE/EXPORTACION_WEB/SS/CIUDADMAGAZINE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>EL GARAGE</t>
+          <t>MULTIVISION HD</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/ELGARAGE/EXPORTACION_WEB/SS/ELGARAGE_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/MULTIVISIONHD/EXPORTACION_WEB/SS/MULTIVISIONHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY TURBO</t>
+          <t>10 DE SALTA</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/DISCOVERYTURBO/EXPORTACION_WEB/SS/DISCOVERYTURBO_t-290x163.png</t>
+          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/10DESALTA/EXPORTACION_WEB/SS/10DESALTA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>PX TV HD</t>
+          <t>CANAL 7 CATAMARCA</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/PXTVHD/EXPORTACION_WEB/SS/PXTVHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CANAL7CATAMARCA/EXPORTACION_WEB/SS/CANAL7CATAMARCA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>ESPN PREMIUM</t>
+          <t>T5 SATELITAL</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/ESPNPREMIUM/EXPORTACION_WEB/SS/ESPNPREMIUM_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/T5SATELITAL/EXPORTACION_WEB/SS/T5SATELITAL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>TNT SPORTS ARGENTINA</t>
+          <t>CANAL 7 JUJUY</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/TNTSPORTSARGENTINA/EXPORTACION_WEB/SS/TNTSPORTSARGENTINA_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CANAL7JUJUY/EXPORTACION_WEB/SS/CANAL7JUJUY_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY KIDS CHANNEL</t>
+          <t>CANAL 10 CÓRDOBA</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/DISCOVERYKIDSCHANNEL/EXPORTACION_WEB/SS/DISCOVERYKIDSCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/CANAL10CRDOBA/EXPORTACION_WEB/SS/CANAL10CRDOBA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>90</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>DISNEY CHANNEL</t>
+          <t>SONY CHANNEL</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/DISNEYCHANNEL/EXPORTACION_WEB/SS/DISNEYCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/SONYCHANNEL/EXPORTACION_WEB/SS/SONYCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>100</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>DISNEY JUNIOR</t>
+          <t>CLARO SPORTS</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/DISNEYJUNIOR/EXPORTACION_WEB/SS/DISNEYJUNIOR_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CLAROSPORTS/EXPORTACION_WEB/SS/CLAROSPORTS_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>TEENNICK</t>
+          <t>ESPN NEW</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/TEENNICK/EXPORTACION_WEB/SS/TEENNICK_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/ESPNNEW/EXPORTACION_WEB/SS/ESPNNEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>107</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>NICK JR HD</t>
+          <t>ESPN 2 NEW</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/NICKJRHD/EXPORTACION_WEB/SS/NICKJRHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/ESPN2NEW/EXPORTACION_WEB/SS/ESPN2NEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>NICK HD ARG</t>
+          <t>ESPN 3</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/NICKHDARG/EXPORTACION_WEB/SS/NICKHDARG_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/ESPN3/EXPORTACION_WEB/SS/ESPN3_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>109</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>CARTOON NETWORK HD</t>
+          <t>ESPN 4</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CARTOONNETWORKHD/EXPORTACION_WEB/SS/CARTOONNETWORKHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/ESPN4/EXPORTACION_WEB/SS/ESPN4_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>110</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>PAKA PAKA</t>
+          <t>FOX SPORTS NEW</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/PAKAPAKA/EXPORTACION_WEB/SS/PAKAPAKA_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/FOXSPORTSNEW/EXPORTACION_WEB/SS/FOXSPORTSNEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>111</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>CARTOONITO</t>
+          <t>FOX SPORTS 2 NEW</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/CARTOONITO/EXPORTACION_WEB/SS/CARTOONITO_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/FOXSPORTS2NEW/EXPORTACION_WEB/SS/FOXSPORTS2NEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>112</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>PLIM PLIM</t>
+          <t>FOX SPORTS 3 NEW</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/PLIMPLIM/EXPORTACION_WEB/SS/PLIMPLIM_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/FOXSPORTS3NEW/EXPORTACION_WEB/SS/FOXSPORTS3NEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>113</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>TOONCAST</t>
+          <t>DeporTV HD</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/TOONCAST/EXPORTACION_WEB/SS/TOONCAST_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DEPORTVHD/EXPORTACION_WEB/SS/DEPORTVHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>114</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>BABY TV</t>
+          <t>EL GARAGE</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/BABYTV/EXPORTACION_WEB/SS/BABYTV_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/ELGARAGE/EXPORTACION_WEB/SS/ELGARAGE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>CLARO CINEMA HD</t>
+          <t>DISCOVERY TURBO</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CLAROCINEMAHD/EXPORTACION_WEB/SS/CLAROCINEMAHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DISCOVERYTURBO/EXPORTACION_WEB/SS/DISCOVERYTURBO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>118</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERYIDHD</t>
+          <t>PX TV HD</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/DISCOVERYIDHD/EXPORTACION_WEB/SS/DISCOVERYIDHD_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/PXTVHD/EXPORTACION_WEB/SS/PXTVHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>STAR CHANNEL</t>
+          <t>ESPN PREMIUM</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/STARCHANNEL/EXPORTACION_WEB/SS/STARCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/ESPNPREMIUM/EXPORTACION_WEB/SS/ESPNPREMIUM_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>303</t>
+          <t>121</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>FX HD</t>
+          <t>TNT SPORTS ARGENTINA</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/FXHD/EXPORTACION_WEB/SS/FXHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/TNTSPORTSARGENTINA/EXPORTACION_WEB/SS/TNTSPORTSARGENTINA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>201</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>SONY MOVIES HD</t>
+          <t>DISCOVERY KIDS CHANNEL</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/SONYMOVIESHD/EXPORTACION_WEB/SS/SONYMOVIESHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/DISCOVERYKIDSCHANNEL/EXPORTACION_WEB/SS/DISCOVERYKIDSCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>202</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>CINECANAL HD</t>
+          <t>DISNEY CHANNEL</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CINECANALHD/EXPORTACION_WEB/SS/CINECANALHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/DISNEYCHANNEL/EXPORTACION_WEB/SS/DISNEYCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>TCM</t>
+          <t>DISNEY JUNIOR</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/TCM/EXPORTACION_WEB/SS/TCM_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/DISNEYJUNIOR/EXPORTACION_WEB/SS/DISNEYJUNIOR_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>309</t>
+          <t>206</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>TNT HD</t>
+          <t>TEENNICK</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/TNTHD/EXPORTACION_WEB/SS/TNTHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/TEENNICK/EXPORTACION_WEB/SS/TEENNICK_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>310</t>
+          <t>207</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>TNT SERIES HD</t>
+          <t>NICK JR HD</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/TNTSERIESHD/EXPORTACION_WEB/SS/TNTSERIESHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/NICKJRHD/EXPORTACION_WEB/SS/NICKJRHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>311</t>
+          <t>208</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>SPACE HD</t>
+          <t>NICK HD ARG</t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/SPACEHD/EXPORTACION_WEB/SS/SPACEHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/NICKHDARG/EXPORTACION_WEB/SS/NICKHDARG_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>211</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>AE MUNDO HD</t>
+          <t>CARTOON NETWORK HD</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/AEMUNDOHD/EXPORTACION_WEB/SS/AEMUNDOHD_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CARTOONNETWORKHD/EXPORTACION_WEB/SS/CARTOONNETWORKHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>AXN HD</t>
+          <t>PAKA PAKA</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/AXNHD/EXPORTACION_WEB/SS/AXNHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/PAKAPAKA/EXPORTACION_WEB/SS/PAKAPAKA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>317</t>
+          <t>213</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>CINEMAX HD</t>
+          <t>CARTOONITO</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/CINEMAXHD/EXPORTACION_WEB/SS/CINEMAXHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/CARTOONITO/EXPORTACION_WEB/SS/CARTOONITO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>318</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>SONY CHANNEL</t>
+          <t>TOONCAST</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/SONYCHANNEL/EXPORTACION_WEB/SS/SONYCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/TOONCAST/EXPORTACION_WEB/SS/TOONCAST_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>216</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>WARNER CHANNEL HD</t>
+          <t>BABY TV</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/WARNERCHANNELHD/EXPORTACION_WEB/SS/WARNERCHANNELHD_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/BABYTV/EXPORTACION_WEB/SS/BABYTV_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>299</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL HD</t>
+          <t>CLARO CINEMA HD</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/UNIVERSALHD/EXPORTACION_WEB/SS/UNIVERSALHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/CLAROCINEMAHD/EXPORTACION_WEB/SS/CLAROCINEMAHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>300</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>DISCOVERYIDHD</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/USA/EXPORTACION_WEB/SS/USA_t-290x163.png</t>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/DISCOVERYIDHD/EXPORTACION_WEB/SS/DISCOVERYIDHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>322</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>STUDIO UNIVERSAL</t>
+          <t>STAR CHANNEL</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/STUDIOUNIVERSAL/EXPORTACION_WEB/SS/STUDIOUNIVERSAL_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/STARCHANNEL/EXPORTACION_WEB/SS/STARCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>323</t>
+          <t>303</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>TELEMUNDO</t>
+          <t>FX HD</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/TELEMUNDO/EXPORTACION_WEB/SS/TELEMUNDO_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/FXHD/EXPORTACION_WEB/SS/FXHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>326</t>
+          <t>308</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>TVE HD</t>
+          <t>TCM</t>
         </is>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/RTVE/PELICULAS/TVEHD/EXPORTACION_WEB/SS/TVEHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/TCM/EXPORTACION_WEB/SS/TCM_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>309</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>STAR TVE HD</t>
+          <t>TNT HD</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/RTVE/PELICULAS/STARTVEHD/EXPORTACION_WEB/SS/STARTVEHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/TNTHD/EXPORTACION_WEB/SS/TNTHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>328</t>
+          <t>310</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>A3SERIES</t>
+          <t>TNT SERIES HD</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn3.clarovideo.net/ATRESPLAYER/PELICULAS/A3SERIES/EXPORTACION_WEB/SS/A3SERIES_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/TNTSERIESHD/EXPORTACION_WEB/SS/TNTSERIESHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>311</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>AMC HD</t>
+          <t>SPACE HD</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/AMCHD/EXPORTACION_WEB/SS/AMCHD_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/SPACEHD/EXPORTACION_WEB/SS/SPACEHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>315</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>EUROPA EUROPA HD</t>
+          <t>AE MUNDO HD</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/EUROPAEUROPAHD/EXPORTACION_WEB/SS/EUROPAEUROPAHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/AEMUNDOHD/EXPORTACION_WEB/SS/AEMUNDOHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>316</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>FILM AND ARTS HD</t>
+          <t>AXN HD</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/FILMANDARTSHD/EXPORTACION_WEB/SS/FILMANDARTSHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/AXNHD/EXPORTACION_WEB/SS/AXNHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>339</t>
+          <t>317</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>PARAMOUNT CHANNEL HD</t>
+          <t>CINEMAX HD</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/PARAMOUNTCHANNELHD/EXPORTACION_WEB/SS/PARAMOUNTCHANNELHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/CINEMAXHD/EXPORTACION_WEB/SS/CINEMAXHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>319</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>COMEDY CENTRAL HD</t>
+          <t>WARNER CHANNEL HD</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/COMEDYCENTRALHD/EXPORTACION_WEB/SS/COMEDYCENTRALHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/WARNERCHANNELHD/EXPORTACION_WEB/SS/WARNERCHANNELHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>320</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>CINEAR</t>
+          <t>UNIVERSAL HD</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CINEAR/EXPORTACION_WEB/SS/CINEAR_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/UNIVERSALHD/EXPORTACION_WEB/SS/UNIVERSALHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>321</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>RCN TELENOVELAS</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/RCNTELENOVELAS/EXPORTACION_WEB/SS/RCNTELENOVELAS_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/USA/EXPORTACION_WEB/SS/USA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>322</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>PASIONES HD</t>
+          <t>STUDIO UNIVERSAL</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/PASIONESHD/EXPORTACION_WEB/SS/PASIONESHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/STUDIOUNIVERSAL/EXPORTACION_WEB/SS/STUDIOUNIVERSAL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>323</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>CANAL CLARO HD</t>
+          <t>TELEMUNDO</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/CANALCLAROHD/EXPORTACION_WEB/SS/CANALCLAROHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/TELEMUNDO/EXPORTACION_WEB/SS/TELEMUNDO_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>325</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY HOME AND HEALTH CHANNEL</t>
+          <t>VOLVER</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/DISCOVERYHOMEANDHEALTHCHANNEL/EXPORTACION_WEB/SS/DISCOVERYHOMEANDHEALTHCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/VOLVER/EXPORTACION_WEB/SS/VOLVER_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>326</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>TLC CHANNEL</t>
+          <t>TVE HD</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/TLCCHANNEL/EXPORTACION_WEB/SS/TLCCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/TVEHD/EXPORTACION_WEB/SS/TVEHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>327</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>HOLA TV</t>
+          <t>STAR TVE HD</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn9.clarovideo.net/ATRESPLAYER/PELICULAS/HOLATV/EXPORTACION_WEB/SS/HOLATV_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/STARTVEHD/EXPORTACION_WEB/SS/STARTVEHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>328</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>El GOURMET CHANNEL</t>
+          <t>A3SERIES</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/ELGOURMETCHANNEL/EXPORTACION_WEB/SS/ELGOURMETCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/A3SERIES/EXPORTACION_WEB/SS/A3SERIES_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>374</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
         <is>
-          <t>MÁS CHIC HD</t>
+          <t>AMC HD</t>
         </is>
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/MSCHICHD/EXPORTACION_WEB/SS/MSCHICHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/AMCHD/EXPORTACION_WEB/SS/AMCHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>332</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>E ENTERTAINMENT HD</t>
+          <t>EUROPA EUROPA HD</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/EENTERTAINMENTHD/EXPORTACION_WEB/SS/EENTERTAINMENTHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/EUROPAEUROPAHD/EXPORTACION_WEB/SS/EUROPAEUROPAHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>333</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>LIFETIME NEW</t>
+          <t>FILM AND ARTS HD</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/LIFETIMENEW/EXPORTACION_WEB/SS/LIFETIMENEW_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/FILMANDARTSHD/EXPORTACION_WEB/SS/FILMANDARTSHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>339</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>FOODNETWORK HD</t>
+          <t>PARAMOUNT CHANNEL HD</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/FOODNETWORKHD/EXPORTACION_WEB/SS/FOODNETWORKHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/PARAMOUNTCHANNELHD/EXPORTACION_WEB/SS/PARAMOUNTCHANNELHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>ANIMAL PLANET HD</t>
+          <t>COMEDY CENTRAL HD</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/ANIMALPLANETHD/EXPORTACION_WEB/SS/ANIMALPLANETHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/COMEDYCENTRALHD/EXPORTACION_WEB/SS/COMEDYCENTRALHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>401</t>
+          <t>341</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY CHANNEL NEW HD</t>
+          <t>CINEAR</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/DISCOVERYCHANNELNEWHD/EXPORTACION_WEB/SS/DISCOVERYCHANNELNEWHD_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CINEAR/EXPORTACION_WEB/SS/CINEAR_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>350</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>HOME AND GARDEN</t>
+          <t>RCN TELENOVELAS</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/HOMEANDGARDEN/EXPORTACION_WEB/SS/HOMEANDGARDEN_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/RCNTELENOVELAS/EXPORTACION_WEB/SS/RCNTELENOVELAS_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY SCIENCE</t>
+          <t>PASIONES HD</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/DISCOVERYSCIENCE/EXPORTACION_WEB/SS/DISCOVERYSCIENCE_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/PASIONESHD/EXPORTACION_WEB/SS/PASIONESHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>405</t>
+          <t>369</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY WORLD HD</t>
+          <t>CANAL CLARO HD</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/DISCOVERYWORLDHD/EXPORTACION_WEB/SS/DISCOVERYWORLDHD_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/CANALCLAROHD/EXPORTACION_WEB/SS/CANALCLAROHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>406</t>
+          <t>370</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>DISCOVERY THEATER HD</t>
+          <t>DISCOVERY HOME AND HEALTH CHANNEL</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/DISCOVERYTHEATERHD/EXPORTACION_WEB/SS/DISCOVERYTHEATERHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DISCOVERYHOMEANDHEALTHCHANNEL/EXPORTACION_WEB/SS/DISCOVERYHOMEANDHEALTHCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>371</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>NATIONAL GEOGRAPHIC HD</t>
+          <t>TLC CHANNEL</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/NATIONALGEOGRAPHICHD/EXPORTACION_WEB/SS/NATIONALGEOGRAPHICHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/TLCCHANNEL/EXPORTACION_WEB/SS/TLCCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>414</t>
+          <t>372</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>HISTORY 2</t>
+          <t>HOLA HD</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/HISTORY2/EXPORTACION_WEB/SS/HISTORY2_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/HOLAHD/EXPORTACION_WEB/SS/HOLAHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>373</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>HISTORY CHANNEL HD</t>
+          <t>El GOURMET CHANNEL</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/HISTORYCHANNELHD/EXPORTACION_WEB/SS/HISTORYCHANNELHD_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/ELGOURMETCHANNEL/EXPORTACION_WEB/SS/ELGOURMETCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>417</t>
+          <t>374</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>UNIFE</t>
+          <t>MÁS CHIC HD</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/UNIFE/EXPORTACION_WEB/SS/UNIFE_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/MSCHICHD/EXPORTACION_WEB/SS/MSCHICHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>471</t>
+          <t>375</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>CANAL RURAL</t>
+          <t>E ENTERTAINMENT HD</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/CANALRURAL/EXPORTACION_WEB/SS/CANALRURAL_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/EENTERTAINMENTHD/EXPORTACION_WEB/SS/EENTERTAINMENTHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>472</t>
+          <t>380</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>CHACRA TV</t>
+          <t>LIFETIME NEW</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/CHACRATV/EXPORTACION_WEB/SS/CHACRATV_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/LIFETIMENEW/EXPORTACION_WEB/SS/LIFETIMENEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>502</t>
+          <t>381</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
         <is>
-          <t>CNN EN ESPAÑOL</t>
+          <t>FOODNETWORK HD</t>
         </is>
       </c>
       <c r="C101" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CNNENESPAOL/EXPORTACION_WEB/SS/CNNENESPAOL_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/FOODNETWORKHD/EXPORTACION_WEB/SS/FOODNETWORKHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>503</t>
+          <t>400</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>CNN INTERNACIONAL</t>
+          <t>ANIMAL PLANET HD</t>
         </is>
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CNNINTERNACIONAL/EXPORTACION_WEB/SS/CNNINTERNACIONAL_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/ANIMALPLANETHD/EXPORTACION_WEB/SS/ANIMALPLANETHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>507</t>
+          <t>401</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
         <is>
-          <t>FRANCE24 HD</t>
+          <t>DISCOVERY CHANNEL HD</t>
         </is>
       </c>
       <c r="C103" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/FRANCE24HD/EXPORTACION_WEB/SS/FRANCE24HD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/DISCOVERYCHANNELHD/EXPORTACION_WEB/SS/DISCOVERYCHANNELHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>509</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>DW TV</t>
+          <t>HOME AND GARDEN</t>
         </is>
       </c>
       <c r="C104" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/DWTV/EXPORTACION_WEB/SS/DWTV_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/HOMEANDGARDEN/EXPORTACION_WEB/SS/HOMEANDGARDEN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>404</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
         <is>
-          <t>RAI</t>
+          <t>DISCOVERY SCIENCE</t>
         </is>
       </c>
       <c r="C105" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/RAI/EXPORTACION_WEB/SS/RAI_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/DISCOVERYSCIENCE/EXPORTACION_WEB/SS/DISCOVERYSCIENCE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>512</t>
+          <t>405</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>DISCOVERY WORLD</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/UCL/EXPORTACION_WEB/SS/UCL_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DISCOVERYWORLD/EXPORTACION_WEB/SS/DISCOVERYWORLD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>513</t>
+          <t>406</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
         <is>
-          <t>ARGENTINISIMA SATELITAL</t>
+          <t>DISCOVERY THEATER HD</t>
         </is>
       </c>
       <c r="C107" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/ARGENTINISIMASATELITAL/EXPORTACION_WEB/SS/ARGENTINISIMASATELITAL_t-290x163.png</t>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/DISCOVERYTHEATERHD/EXPORTACION_WEB/SS/DISCOVERYTHEATERHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>515</t>
+          <t>412</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t>24H TVE</t>
+          <t>NATIONAL GEOGRAPHIC HD</t>
         </is>
       </c>
       <c r="C108" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/RTVE/PELICULAS/24HTVE/EXPORTACION_WEB/SS/24HTVE_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/NATIONALGEOGRAPHICHD/EXPORTACION_WEB/SS/NATIONALGEOGRAPHICHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>414</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
         <is>
-          <t>INTI HD</t>
+          <t>HISTORY 2</t>
         </is>
       </c>
       <c r="C109" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/INTIHD/EXPORTACION_WEB/SS/INTIHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/HISTORY2/EXPORTACION_WEB/SS/HISTORY2_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>415</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
         <is>
-          <t>MARÍA VISIÓN</t>
+          <t>HISTORY CHANNEL HD</t>
         </is>
       </c>
       <c r="C110" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/MARAVISIN/EXPORTACION_WEB/SS/MARAVISIN_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/HISTORYCHANNELHD/EXPORTACION_WEB/SS/HISTORYCHANNELHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>521</t>
+          <t>502</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
         <is>
-          <t>EWTN</t>
+          <t>CNN EN ESPAÑOL</t>
         </is>
       </c>
       <c r="C111" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/EWTN/EXPORTACION_WEB/SS/EWTN_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CNNENESPAOL/EXPORTACION_WEB/SS/CNNENESPAOL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>503</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>ENLACE</t>
+          <t>CNN INTERNACIONAL</t>
         </is>
       </c>
       <c r="C112" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/ENLACE/EXPORTACION_WEB/SS/ENLACE_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CNNINTERNACIONAL/EXPORTACION_WEB/SS/CNNINTERNACIONAL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>523</t>
+          <t>507</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>EL SEMBRADOR</t>
+          <t>FRANCE24 HD</t>
         </is>
       </c>
       <c r="C113" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/ELSEMBRADOR/EXPORTACION_WEB/SS/ELSEMBRADOR_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/FRANCE24HD/EXPORTACION_WEB/SS/FRANCE24HD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>509</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
         <is>
-          <t>ORBE 21</t>
+          <t>DW TV</t>
         </is>
       </c>
       <c r="C114" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/ORBE21/EXPORTACION_WEB/SS/ORBE21_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/DWTV/EXPORTACION_WEB/SS/DWTV_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>511</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
         <is>
-          <t>CLAROTV ARGENTINA</t>
+          <t>RAI</t>
         </is>
       </c>
       <c r="C115" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/CLAROTVARGENTINA/EXPORTACION_WEB/SS/CLAROTVARGENTINA_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/RAI/EXPORTACION_WEB/SS/RAI_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>512</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
         <is>
-          <t>CONCERT CHANNEL HD</t>
+          <t>UCL</t>
         </is>
       </c>
       <c r="C116" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CONCERTCHANNELHD/EXPORTACION_WEB/SS/CONCERTCHANNELHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/UCL/EXPORTACION_WEB/SS/UCL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>553</t>
+          <t>513</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
         <is>
-          <t>CANAL DE LA MÚSICA</t>
+          <t>ARGENTINISIMA SATELITAL</t>
         </is>
       </c>
       <c r="C117" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/CANALDELAMSICA/EXPORTACION_WEB/SS/CANALDELAMSICA_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/ARGENTINISIMASATELITAL/EXPORTACION_WEB/SS/ARGENTINISIMASATELITAL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>554</t>
+          <t>515</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>MTV HD</t>
+          <t>24H TVE</t>
         </is>
       </c>
       <c r="C118" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/MTVHD/EXPORTACION_WEB/SS/MTVHD_t-290x163.png</t>
+          <t>https://clarovideocdn2.clarovideo.net/RTVE/PELICULAS/24HTVE/EXPORTACION_WEB/SS/24HTVE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>517</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
         <is>
-          <t>MTV HITS</t>
+          <t>INTI HD</t>
         </is>
       </c>
       <c r="C119" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/MTVHITS/EXPORTACION_WEB/SS/MTVHITS_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/INTIHD/EXPORTACION_WEB/SS/INTIHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>556</t>
+          <t>520</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
         <is>
-          <t>MTV LIVE HD</t>
+          <t>MARÍA VISIÓN</t>
         </is>
       </c>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/MTVLIVEHD/EXPORTACION_WEB/SS/MTVLIVEHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/MARAVISIN/EXPORTACION_WEB/SS/MARAVISIN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>557</t>
+          <t>521</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
         <is>
-          <t>MTV CLUB</t>
+          <t>EWTN</t>
         </is>
       </c>
       <c r="C121" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/MTVCLUB/EXPORTACION_WEB/SS/MTVCLUB_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/EWTN/EXPORTACION_WEB/SS/EWTN_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>558</t>
+          <t>522</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
         <is>
-          <t>MTV 00's</t>
+          <t>ENLACE</t>
         </is>
       </c>
       <c r="C122" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/MTV00S/EXPORTACION_WEB/SS/MTV00S_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/ENLACE/EXPORTACION_WEB/SS/ENLACE_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>559</t>
+          <t>523</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
         <is>
-          <t>MTV 80</t>
+          <t>EL SEMBRADOR</t>
         </is>
       </c>
       <c r="C123" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/MTV80/EXPORTACION_WEB/SS/MTV80_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/ELSEMBRADOR/EXPORTACION_WEB/SS/ELSEMBRADOR_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>NICKMUSIC</t>
+          <t>ORBE 21</t>
         </is>
       </c>
       <c r="C124" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/NICKMUSIC/EXPORTACION_WEB/SS/NICKMUSIC_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/ORBE21/EXPORTACION_WEB/SS/ORBE21_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>562</t>
+          <t>551</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
         <is>
-          <t>HTV</t>
+          <t>CONCERT CHANNEL HD</t>
         </is>
       </c>
       <c r="C125" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/HTV/EXPORTACION_WEB/SS/HTV_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/CONCERTCHANNELHD/EXPORTACION_WEB/SS/CONCERTCHANNELHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>552</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
         <is>
-          <t>HBO FAMILY CHANNEL</t>
+          <t>QUIERO MÚSICA</t>
         </is>
       </c>
       <c r="C126" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBOFAMILYCHANNEL/EXPORTACION_WEB/SS/HBOFAMILYCHANNEL_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/PELICULAS/QUIEROMSICA/EXPORTACION_WEB/SS/QUIEROMSICA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>602</t>
+          <t>553</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
         <is>
-          <t>HBO HD</t>
+          <t>CANAL DE LA MÚSICA</t>
         </is>
       </c>
       <c r="C127" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn9.clarovideo.net/HBO/PELICULAS/HBOHD/EXPORTACION_WEB/SS/HBOHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/CANALDELAMSICA/EXPORTACION_WEB/SS/CANALDELAMSICA_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>603</t>
+          <t>554</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
         <is>
-          <t>HBOMUNDI</t>
+          <t>MTV HD</t>
         </is>
       </c>
       <c r="C128" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn5.clarovideo.net/HBO/PELICULAS/HBOMUNDI/EXPORTACION_WEB/SS/HBOMUNDI_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/PELICULAS/MTVHD/EXPORTACION_WEB/SS/MTVHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>604</t>
+          <t>555</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
         <is>
-          <t>HBO PLUS HD</t>
+          <t>MTV HITS</t>
         </is>
       </c>
       <c r="C129" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn7.clarovideo.net/HBO/PELICULAS/HBOPLUSHD/EXPORTACION_WEB/SS/HBOPLUSHD_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/MTVHITS/EXPORTACION_WEB/SS/MTVHITS_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>605</t>
+          <t>556</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
         <is>
-          <t>HBO SIGNATURE HD NEW</t>
+          <t>MTV LIVE HD</t>
         </is>
       </c>
       <c r="C130" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn3.clarovideo.net/HBO/PELICULAS/HBOSIGNATUREHDNEW/EXPORTACION_WEB/SS/HBOSIGNATUREHDNEW_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/MTVLIVEHD/EXPORTACION_WEB/SS/MTVLIVEHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>606</t>
+          <t>557</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
         <is>
-          <t>HBO 2 HD</t>
+          <t>MTV CLUB</t>
         </is>
       </c>
       <c r="C131" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBO2HD/EXPORTACION_WEB/SS/HBO2HD_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/MTVCLUB/EXPORTACION_WEB/SS/MTVCLUB_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>558</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
         <is>
-          <t>HBOXTREME</t>
+          <t>MTV 00's</t>
         </is>
       </c>
       <c r="C132" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn7.clarovideo.net/HBO/PELICULAS/HBOXTREME/EXPORTACION_WEB/SS/HBOXTREME_t-290x163.png</t>
+          <t>https://clarovideocdn4.clarovideo.net/CVPERU/PELICULAS/MTV00S/EXPORTACION_WEB/SS/MTV00S_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>611</t>
+          <t>559</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
         <is>
-          <t>HBOPOP</t>
+          <t>MTV 80</t>
         </is>
       </c>
       <c r="C133" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBOPOP/EXPORTACION_WEB/SS/HBOPOP_t-290x163.png</t>
+          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/MTV80/EXPORTACION_WEB/SS/MTV80_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>627</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL PREMIERE ESTE HD</t>
+          <t>NICKMUSIC</t>
         </is>
       </c>
       <c r="C134" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/UNIVERSALPREMIEREESTEHD/EXPORTACION_WEB/SS/UNIVERSALPREMIEREESTEHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/NICKMUSIC/EXPORTACION_WEB/SS/NICKMUSIC_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>628</t>
+          <t>562</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL CINEMA HD</t>
+          <t>HTV</t>
         </is>
       </c>
       <c r="C135" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCINEMAHD/EXPORTACION_WEB/SS/UNIVERSALCINEMAHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/HTV/EXPORTACION_WEB/SS/HTV_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>629</t>
+          <t>601</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL COMEDY HD</t>
+          <t>HBO FAMILY CHANNEL</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCOMEDYHD/EXPORTACION_WEB/SS/UNIVERSALCOMEDYHD_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBOFAMILYCHANNEL/EXPORTACION_WEB/SS/HBOFAMILYCHANNEL_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>630</t>
+          <t>602</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL CRIME ESTE HD</t>
+          <t>HBO HD</t>
         </is>
       </c>
       <c r="C137" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCRIMEESTEHD/EXPORTACION_WEB/SS/UNIVERSALCRIMEESTEHD_t-290x163.png</t>
+          <t>https://clarovideocdn9.clarovideo.net/HBO/PELICULAS/HBOHD/EXPORTACION_WEB/SS/HBOHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>631</t>
+          <t>603</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>UNIVERSAL REALITY HD</t>
+          <t>HBOMUNDI</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/UNIVERSALREALITYHD/EXPORTACION_WEB/SS/UNIVERSALREALITYHD_t-290x163.png</t>
+          <t>https://clarovideocdn5.clarovideo.net/HBO/PELICULAS/HBOMUNDI/EXPORTACION_WEB/SS/HBOMUNDI_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>802</t>
+          <t>604</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
         <is>
-          <t>PENTHOUSE</t>
+          <t>HBO PLUS HD</t>
         </is>
       </c>
       <c r="C139" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/PENTHOUSE/EXPORTACION_WEB/SS/PENTHOUSE_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/HBO/PELICULAS/HBOPLUSHD/EXPORTACION_WEB/SS/HBOPLUSHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>803</t>
+          <t>605</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>PLAYBOY HD</t>
+          <t>HBO SIGNATURE HD NEW</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn0.clarovideo.net/CVPERU/PELICULAS/PLAYBOYHD/EXPORTACION_WEB/SS/PLAYBOYHD_t-290x163.png</t>
+          <t>https://clarovideocdn3.clarovideo.net/HBO/PELICULAS/HBOSIGNATUREHDNEW/EXPORTACION_WEB/SS/HBOSIGNATUREHDNEW_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>804</t>
+          <t>606</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
         <is>
-          <t>SEXTREME</t>
+          <t>HBO 2 HD</t>
         </is>
       </c>
       <c r="C141" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/SEXTREME/EXPORTACION_WEB/SS/SEXTREME_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBO2HD/EXPORTACION_WEB/SS/HBO2HD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>805</t>
+          <t>610</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>VENUS</t>
+          <t>HBOXTREME</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/VENUS/EXPORTACION_WEB/SS/VENUS_t-290x163.png</t>
+          <t>https://clarovideocdn7.clarovideo.net/HBO/PELICULAS/HBOXTREME/EXPORTACION_WEB/SS/HBOXTREME_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>611</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
         <is>
-          <t>ANTENA 3 INTERNACIONAL</t>
+          <t>HBOPOP</t>
         </is>
       </c>
       <c r="C143" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn7.clarovideo.net/ATRESPLAYER/PELICULAS/ANTENA3INTERNACIONAL/EXPORTACION_WEB/SS/ANTENA3INTERNACIONAL_t-290x163.png</t>
+          <t>https://clarovideocdn1.clarovideo.net/HBO/PELICULAS/HBOPOP/EXPORTACION_WEB/SS/HBOPOP_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>627</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>ATRESCINE</t>
+          <t>UNIVERSAL PREMIERE ESTE HD</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn5.clarovideo.net/ATRESPLAYER/PELICULAS/ATRESCINE/EXPORTACION_WEB/SS/ATRESCINE_t-290x163.png</t>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/UNIVERSALPREMIEREESTEHD/EXPORTACION_WEB/SS/UNIVERSALPREMIEREESTEHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>628</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
         <is>
-          <t>CLAN HD</t>
+          <t>UNIVERSAL CINEMA HD</t>
         </is>
       </c>
       <c r="C145" s="2" t="inlineStr">
         <is>
-          <t>https://clarovideocdn2.clarovideo.net/RTVE/PELICULAS/CLANHD/EXPORTACION_WEB/SS/CLANHD_t-290x163.png</t>
+          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCINEMAHD/EXPORTACION_WEB/SS/UNIVERSALCINEMAHD_t-290x163.png</t>
         </is>
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="3" t="inlineStr">
+      <c r="A146" s="2" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="B146" s="2" t="inlineStr">
+        <is>
+          <t>UNIVERSAL COMEDY HD</t>
+        </is>
+      </c>
+      <c r="C146" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn6.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCOMEDYHD/EXPORTACION_WEB/SS/UNIVERSALCOMEDYHD_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
+      </c>
+      <c r="B147" s="2" t="inlineStr">
+        <is>
+          <t>UNIVERSAL CRIME ESTE HD</t>
+        </is>
+      </c>
+      <c r="C147" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/UNIVERSALCRIMEESTEHD/EXPORTACION_WEB/SS/UNIVERSALCRIMEESTEHD_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="inlineStr">
+        <is>
+          <t>631</t>
+        </is>
+      </c>
+      <c r="B148" s="2" t="inlineStr">
+        <is>
+          <t>UNIVERSAL REALITY HD</t>
+        </is>
+      </c>
+      <c r="C148" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/UNIVERSALREALITYHD/EXPORTACION_WEB/SS/UNIVERSALREALITYHD_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="inlineStr">
+        <is>
+          <t>802</t>
+        </is>
+      </c>
+      <c r="B149" s="2" t="inlineStr">
+        <is>
+          <t>PENTHOUSE</t>
+        </is>
+      </c>
+      <c r="C149" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/PENTHOUSE/EXPORTACION_WEB/SS/PENTHOUSE_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="inlineStr">
+        <is>
+          <t>803</t>
+        </is>
+      </c>
+      <c r="B150" s="2" t="inlineStr">
+        <is>
+          <t>PLAYBOY HD</t>
+        </is>
+      </c>
+      <c r="C150" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn3.clarovideo.net/PELICULAS/PLAYBOYHD/EXPORTACION_WEB/SS/PLAYBOYHD_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="inlineStr">
+        <is>
+          <t>804</t>
+        </is>
+      </c>
+      <c r="B151" s="2" t="inlineStr">
+        <is>
+          <t>SEXTREME</t>
+        </is>
+      </c>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn1.clarovideo.net/PELICULAS/SEXTREME/EXPORTACION_WEB/SS/SEXTREME_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="inlineStr">
+        <is>
+          <t>805</t>
+        </is>
+      </c>
+      <c r="B152" s="2" t="inlineStr">
+        <is>
+          <t>VENUS</t>
+        </is>
+      </c>
+      <c r="C152" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn2.clarovideo.net/CVPERU/PELICULAS/VENUS/EXPORTACION_WEB/SS/VENUS_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="inlineStr">
+        <is>
+          <t>902</t>
+        </is>
+      </c>
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t>AMÉRICA MENDOZA</t>
+        </is>
+      </c>
+      <c r="C153" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn8.clarovideo.net/CVPERU/PELICULAS/AMRICAMENDOZA/EXPORTACION_WEB/SS/AMRICAMENDOZA_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="inlineStr">
+        <is>
+          <t>911</t>
+        </is>
+      </c>
+      <c r="B154" s="2" t="inlineStr">
+        <is>
+          <t>CANAL 11 SALTA</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="inlineStr">
+        <is>
+          <t>https://clarovideocdn9.clarovideo.net/PELICULAS/CANAL11SALTA/EXPORTACION_WEB/SS/CANAL11SALTA_t-290x163.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="3" t="inlineStr">
         <is>
           <t>Total de canales:</t>
         </is>
       </c>
-      <c r="B146" s="2" t="n">
-        <v>144</v>
+      <c r="B155" s="2" t="n">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>